<commit_message>
incorrect thread numbers spawned
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8903,10 +8903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK18"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26"/>
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8914,7 +8914,7 @@
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -8939,7 +8939,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9075,41 +9075,8 @@
         <f>T3/1000</f>
         <v>9.9273599999999992E-4</v>
       </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>1.7696E-2</v>
-      </c>
-      <c r="AC3">
-        <v>1.7760000000000001E-2</v>
-      </c>
-      <c r="AD3">
-        <v>1.7663999999999999E-2</v>
-      </c>
-      <c r="AE3">
-        <v>1.7919999999999998E-2</v>
-      </c>
-      <c r="AF3">
-        <v>1.7856E-2</v>
-      </c>
-      <c r="AG3">
-        <v>1.8239999999999999E-2</v>
-      </c>
-      <c r="AH3">
-        <v>1.7728000000000001E-2</v>
-      </c>
-      <c r="AI3">
-        <v>1.7824E-2</v>
-      </c>
-      <c r="AJ3">
-        <v>1.7824E-2</v>
-      </c>
-      <c r="AK3">
-        <v>1.7791999999999999E-2</v>
-      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -9180,14 +9147,8 @@
         <f t="shared" ref="Y4:Y16" si="2">T4/1000</f>
         <v>1.0811500000000001E-3</v>
       </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AB4">
-        <v>1.7919999999999998E-2</v>
-      </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -9258,14 +9219,8 @@
         <f t="shared" si="2"/>
         <v>1.3781399999999999E-3</v>
       </c>
-      <c r="AA5">
-        <v>2</v>
-      </c>
-      <c r="AB5">
-        <v>1.7856E-2</v>
-      </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -9336,14 +9291,8 @@
         <f t="shared" si="2"/>
         <v>1.4769900000000001E-3</v>
       </c>
-      <c r="AA6">
-        <v>3</v>
-      </c>
-      <c r="AB6">
-        <v>1.7728000000000001E-2</v>
-      </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -9414,14 +9363,8 @@
         <f t="shared" si="2"/>
         <v>1.54038E-3</v>
       </c>
-      <c r="AA7">
-        <v>4</v>
-      </c>
-      <c r="AB7">
-        <v>1.84E-2</v>
-      </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -9492,14 +9435,8 @@
         <f t="shared" si="2"/>
         <v>1.6062099999999998E-3</v>
       </c>
-      <c r="AA8">
-        <v>5</v>
-      </c>
-      <c r="AB8">
-        <v>1.8144E-2</v>
-      </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -9570,14 +9507,8 @@
         <f t="shared" si="2"/>
         <v>1.7401299999999999E-3</v>
       </c>
-      <c r="AA9">
-        <v>6</v>
-      </c>
-      <c r="AB9">
-        <v>0.17888000000000001</v>
-      </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16</v>
       </c>
@@ -9648,14 +9579,8 @@
         <f t="shared" si="2"/>
         <v>1.5873900000000002E-3</v>
       </c>
-      <c r="AA10">
-        <v>7</v>
-      </c>
-      <c r="AB10">
-        <v>1.7791999999999999E-2</v>
-      </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -9726,14 +9651,8 @@
         <f t="shared" si="2"/>
         <v>2.2579200000000001E-3</v>
       </c>
-      <c r="AA11">
-        <v>8</v>
-      </c>
-      <c r="AB11">
-        <v>1.4048E-2</v>
-      </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
@@ -9804,14 +9723,8 @@
         <f t="shared" si="2"/>
         <v>6.2351000000000004E-3</v>
       </c>
-      <c r="AA12">
-        <v>9</v>
-      </c>
-      <c r="AB12">
-        <v>1.3856E-2</v>
-      </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>22</v>
       </c>
@@ -9882,14 +9795,8 @@
         <f t="shared" si="2"/>
         <v>2.1696300000000002E-2</v>
       </c>
-      <c r="AA13">
-        <v>10</v>
-      </c>
-      <c r="AB13">
-        <v>1.3856E-2</v>
-      </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>24</v>
       </c>
@@ -9960,11 +9867,8 @@
         <f t="shared" si="2"/>
         <v>8.2067199999999993E-2</v>
       </c>
-      <c r="AA14">
-        <v>11</v>
-      </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>26</v>
       </c>
@@ -10035,11 +9939,8 @@
         <f t="shared" si="2"/>
         <v>0.32700499999999999</v>
       </c>
-      <c r="AA15">
-        <v>12</v>
-      </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>28</v>
       </c>
@@ -10109,19 +10010,6 @@
       <c r="Y16">
         <f t="shared" si="2"/>
         <v>1.30392</v>
-      </c>
-      <c r="AA16">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="27:27" x14ac:dyDescent="0.25">
-      <c r="AA17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="27:27" x14ac:dyDescent="0.25">
-      <c r="AA18">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>